<commit_message>
ACUMORG-16: ACU CI/CD CstCustomization util: fix issues, redesign & functionality extending
Documentation
</commit_message>
<xml_diff>
--- a/ACU Configuration Reference.xlsx
+++ b/ACU Configuration Reference.xlsx
@@ -2007,7 +2007,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2288,6 +2288,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>